<commit_message>
update spending data, eff tax rates computation and bfm steps
</commit_message>
<xml_diff>
--- a/input_data/admin_data/COL/gpinter_COL_2014.xlsx
+++ b/input_data/admin_data/COL/gpinter_COL_2014.xlsx
@@ -447,7 +447,7 @@
         <v>0.73999999999999999</v>
       </c>
       <c r="E2">
-        <v>3.7252902984619199e-09</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -474,7 +474,7 @@
         <v>0.75</v>
       </c>
       <c r="E3">
-        <v>1.86264514923096e-08</v>
+        <v>0.019999999552965164</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -501,7 +501,7 @@
         <v>0.76000000000000001</v>
       </c>
       <c r="E4">
-        <v>1.11758708953857e-07</v>
+        <v>0.029999999329447746</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -528,7 +528,7 @@
         <v>0.77000000000000002</v>
       </c>
       <c r="E5">
-        <v>6.5192580223083496e-07</v>
+        <v>0.039999999105930328</v>
       </c>
       <c r="F5">
         <v>0.999999999999998</v>
@@ -555,7 +555,7 @@
         <v>0.78000000000000003</v>
       </c>
       <c r="E6">
-        <v>3.7737190723419198e-06</v>
+        <v>0.05000000074505806</v>
       </c>
       <c r="F6">
         <v>0.999999999999995</v>
@@ -582,7 +582,7 @@
         <v>0.79000000000000004</v>
       </c>
       <c r="E7">
-        <v>2.1375715732574399e-05</v>
+        <v>0.059999998658895493</v>
       </c>
       <c r="F7">
         <v>0.99999999999996503</v>
@@ -609,7 +609,7 @@
         <v>0.80000000000000004</v>
       </c>
       <c r="E8">
-        <v>0.00011850893497467</v>
+        <v>0.070000000298023224</v>
       </c>
       <c r="F8">
         <v>0.99999999999980504</v>
@@ -636,7 +636,7 @@
         <v>0.81000000000000005</v>
       </c>
       <c r="E9">
-        <v>0.00064313039183616703</v>
+        <v>0.079999998211860657</v>
       </c>
       <c r="F9">
         <v>0.99999999999892397</v>
@@ -663,7 +663,7 @@
         <v>0.81999999999999995</v>
       </c>
       <c r="E10">
-        <v>0.00341851636767388</v>
+        <v>0.090000003576278687</v>
       </c>
       <c r="F10">
         <v>0.99999999999420597</v>
@@ -690,7 +690,7 @@
         <v>0.82999999999999996</v>
       </c>
       <c r="E11">
-        <v>0.0178066231310368</v>
+        <v>0.10000000149011612</v>
       </c>
       <c r="F11">
         <v>0.99999999996945199</v>
@@ -717,7 +717,7 @@
         <v>0.83999999999999997</v>
       </c>
       <c r="E12">
-        <v>0.090937197208404402</v>
+        <v>0.10999999940395355</v>
       </c>
       <c r="F12">
         <v>0.99999999984211796</v>
@@ -744,7 +744,7 @@
         <v>0.84999999999999998</v>
       </c>
       <c r="E13">
-        <v>0.45553392171859802</v>
+        <v>0.11999999731779099</v>
       </c>
       <c r="F13">
         <v>0.99999999919969995</v>

</xml_diff>